<commit_message>
updating product backlog before sprint 2
</commit_message>
<xml_diff>
--- a/sprints/Product Backlog.xlsx
+++ b/sprints/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Corley\Dropbox\Work\_teaching\UWG\Capstone\Spring 2022\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lanthorr\git\Capstone\3\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3838CCD7-8993-4A1E-AB80-532D3D0EC31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A61D2FF-5582-41B6-AC76-AE88504070B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="3630" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>View details of an item in my Trip</t>
-  </si>
-  <si>
     <t>I can remember details about an item (Waypoint, Transportation, Lodging) in my Trip including any custom notes I have added to the item</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>I can update my Trip (e.g., they remove a Waypoint and I decide not to include the Waypoint without them)</t>
+  </si>
+  <si>
+    <t>View details of an item in my Trip with Map data</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +618,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -666,10 +666,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,10 +680,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,10 +694,10 @@
         <v>0</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -708,10 +708,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,38 +722,38 @@
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,10 +764,10 @@
         <v>0</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -778,10 +778,10 @@
         <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -792,10 +792,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -876,10 +876,10 @@
         <v>0</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -890,10 +890,10 @@
         <v>0</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -904,10 +904,10 @@
         <v>0</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -918,10 +918,10 @@
         <v>0</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -932,10 +932,10 @@
         <v>0</v>
       </c>
       <c r="C24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -946,10 +946,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -960,10 +960,10 @@
         <v>0</v>
       </c>
       <c r="C26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -974,10 +974,10 @@
         <v>0</v>
       </c>
       <c r="C27" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -988,15 +988,15 @@
         <v>0</v>
       </c>
       <c r="C28" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>56</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D28">
-    <sortCondition ref="A2:A28"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
+    <sortCondition ref="A2:A29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>